<commit_message>
bcThang => Thêm phục lục PL02C
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982780A8-204E-4E18-90C4-C8ED439011D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321EBFC0-B685-4599-8C4D-4DB7433F4D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
     <sheet name="PL02a" sheetId="8" r:id="rId2"/>
     <sheet name="PL02b" sheetId="1" r:id="rId3"/>
-    <sheet name="PL03a" sheetId="3" r:id="rId4"/>
-    <sheet name="PL03b" sheetId="9" r:id="rId5"/>
-    <sheet name="PL04a" sheetId="2" r:id="rId6"/>
-    <sheet name="PL04b" sheetId="4" r:id="rId7"/>
+    <sheet name="PL02c" sheetId="11" r:id="rId4"/>
+    <sheet name="PL03a" sheetId="3" r:id="rId5"/>
+    <sheet name="PL03b" sheetId="9" r:id="rId6"/>
+    <sheet name="PL04a" sheetId="2" r:id="rId7"/>
+    <sheet name="PL04b" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Mã Tỉnh</t>
   </si>
@@ -141,13 +142,61 @@
   </si>
   <si>
     <t>{filldata}</t>
+  </si>
+  <si>
+    <t>So sánh lượt KCB và chi KCB năm nay với năm trước</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lượt KCB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chi KCB </t>
+  </si>
+  <si>
+    <t>Năm nay</t>
+  </si>
+  <si>
+    <t>năm trước</t>
+  </si>
+  <si>
+    <t>tăng/giảm</t>
+  </si>
+  <si>
+    <t>5=3-4</t>
+  </si>
+  <si>
+    <t>8=6-7</t>
+  </si>
+  <si>
+    <t>Cột A- B02</t>
+  </si>
+  <si>
+    <t>Cột B-B02</t>
+  </si>
+  <si>
+    <t> Cột D-B02-10-2024; từ tháng 1 đến tháng báo cáo</t>
+  </si>
+  <si>
+    <t>  Cột D-B02-10-2023; từ tháng 1 đến tháng báo cáo</t>
+  </si>
+  <si>
+    <t>năm trước - năm nay</t>
+  </si>
+  <si>
+    <t> Cột R-B02-10-2024; từ tháng 1 đến tháng báo cáo</t>
+  </si>
+  <si>
+    <t> Cột R-B02-10-2023; từ tháng 1 đến tháng báo cáo</t>
+  </si>
+  <si>
+    <t>năm trước- năm nay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -293,6 +342,19 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -305,7 +367,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -328,12 +390,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -419,7 +503,30 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,9 +546,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,7 +586,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -585,7 +692,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -727,7 +834,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -875,7 +982,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -950,7 +1057,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -961,6 +1068,194 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D38083D-7A73-433C-93D4-FA213EAF8470}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="18" customWidth="1"/>
+    <col min="3" max="8" width="16.140625" style="18" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>1</v>
+      </c>
+      <c r="B4" s="34">
+        <v>2</v>
+      </c>
+      <c r="C4" s="36">
+        <v>3</v>
+      </c>
+      <c r="D4" s="36">
+        <v>4</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="36">
+        <v>6</v>
+      </c>
+      <c r="G4" s="36">
+        <v>7</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1017,7 +1312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1074,7 +1369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -1133,11 +1428,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bcThang => Thêm phục Lục 03c
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321EBFC0-B685-4599-8C4D-4DB7433F4D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B42FA00-C666-46FE-839E-684AB82B3574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -19,15 +19,16 @@
     <sheet name="PL02c" sheetId="11" r:id="rId4"/>
     <sheet name="PL03a" sheetId="3" r:id="rId5"/>
     <sheet name="PL03b" sheetId="9" r:id="rId6"/>
-    <sheet name="PL04a" sheetId="2" r:id="rId7"/>
-    <sheet name="PL04b" sheetId="4" r:id="rId8"/>
+    <sheet name=" PL03c" sheetId="12" r:id="rId7"/>
+    <sheet name="PL04a" sheetId="2" r:id="rId8"/>
+    <sheet name="PL04b" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
   <si>
     <t>Mã Tỉnh</t>
   </si>
@@ -190,13 +191,67 @@
   </si>
   <si>
     <t>năm trước- năm nay</t>
+  </si>
+  <si>
+    <t>So sánh lượt KCB và chi KCB tháng này với tháng trước</t>
+  </si>
+  <si>
+    <t>Tháng này</t>
+  </si>
+  <si>
+    <t>Tháng trước</t>
+  </si>
+  <si>
+    <t> Cột D-B02-10-2024-tháng này</t>
+  </si>
+  <si>
+    <t>  Cột D-B02-10-2024- tháng trước</t>
+  </si>
+  <si>
+    <t>Tháng này- tháng trước</t>
+  </si>
+  <si>
+    <t> Cột R-B02-10-2024-tháng này</t>
+  </si>
+  <si>
+    <t>  Cột R-B02-10-2024- tháng trước</t>
+  </si>
+  <si>
+    <t>Cột G-B02-10 tháng năy</t>
+  </si>
+  <si>
+    <t>Cột G-B02-10 tháng trước</t>
+  </si>
+  <si>
+    <t>Cột H-B02-10 tháng năy</t>
+  </si>
+  <si>
+    <t>Cột H-B02-10 tháng trước</t>
+  </si>
+  <si>
+    <t>Cột I-B02-10 tháng năy</t>
+  </si>
+  <si>
+    <t>Cột I-B02-10 tháng trước</t>
+  </si>
+  <si>
+    <t>Cột J-B02-10 tháng năy</t>
+  </si>
+  <si>
+    <t>CộtJ-B02-10 tháng trước</t>
+  </si>
+  <si>
+    <t>Cột K-B02-10 tháng năy</t>
+  </si>
+  <si>
+    <t>Cột K-B02-10 tháng trước</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -347,27 +402,27 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -412,12 +467,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -485,12 +601,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -502,30 +612,103 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -845,12 +1028,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="24" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="24" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" style="24" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="24" customWidth="1"/>
@@ -859,59 +1042,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="43" t="s">
         <v>17</v>
       </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="44" t="s">
         <v>23</v>
       </c>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="25" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>1</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="26">
         <v>2</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="26">
         <v>3</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1074,173 +1266,173 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36" style="18" customWidth="1"/>
-    <col min="3" max="8" width="16.140625" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="11.7109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="24" customWidth="1"/>
+    <col min="3" max="8" width="16.7109375" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="39" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="41" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
+      <c r="A4" s="36">
         <v>1</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="36">
         <v>2</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="37">
         <v>3</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="37">
         <v>4</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="37">
         <v>6</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="37">
         <v>7</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+    <row r="5" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="39" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1257,56 +1449,168 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+    </row>
+    <row r="4" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5" s="45"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1370,11 +1674,159 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8040E2C3-F977-4342-8149-0FFE2ADB77F0}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="24" customWidth="1"/>
+    <col min="3" max="8" width="16.7109375" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="41">
+        <v>1</v>
+      </c>
+      <c r="B4" s="41">
+        <v>2</v>
+      </c>
+      <c r="C4" s="41">
+        <v>3</v>
+      </c>
+      <c r="D4" s="41">
+        <v>4</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="41">
+        <v>6</v>
+      </c>
+      <c r="G4" s="41">
+        <v>7</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>

</xml_diff>

<commit_message>
bcThang => PL04B không thấy có dữ liệu vào
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2F7E1C-DDE7-42BA-9C6A-B31B4046659E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF7F16A-B3B8-4D4E-8959-F1B6CC775D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="47">
   <si>
     <t>Mã Tỉnh</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t xml:space="preserve">hạng BV /Tên CSKCB </t>
-  </si>
-  <si>
-    <t>Tên CSYT</t>
   </si>
   <si>
     <t>PHỤ LỤC 01. TÌNH HÌNH SỬ DỤNG DỰ TOÁN THEO HỢP ĐỒNG</t>
@@ -132,10 +129,6 @@
     <t>PHỤ LỤC 04b: SỐ LIỆU SO SÁNH 6 CHỈ SỐ NĐ75 TỪNG CSKCB CỦA THÁNG BÁO CÁO</t>
   </si>
   <si>
-    <t>BQ_THUOC
-(đồng)</t>
-  </si>
-  <si>
     <t>{filldata}</t>
   </si>
   <si>
@@ -176,13 +169,16 @@
   </si>
   <si>
     <t>PHỤ LỤC 03b: SỐ LIỆU SO SÁNH 5 CHỈ SỐ CƠ BẢN TỪNG CSKCB LŨY KẾ NĂM</t>
+  </si>
+  <si>
+    <t>Hạng BV/ Tên CSKCB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -308,12 +304,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
@@ -329,13 +319,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -351,15 +334,21 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -419,16 +408,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -460,28 +459,21 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -496,16 +488,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -535,21 +524,33 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,9 +570,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -609,7 +610,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -715,7 +716,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -857,7 +858,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -868,70 +869,70 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="17" customWidth="1"/>
-    <col min="2" max="2" width="32" style="17" customWidth="1"/>
-    <col min="3" max="4" width="25" style="17" customWidth="1"/>
-    <col min="5" max="5" width="13" style="17" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="11" style="13" customWidth="1"/>
+    <col min="2" max="2" width="32" style="13" customWidth="1"/>
+    <col min="3" max="4" width="25" style="13" customWidth="1"/>
+    <col min="5" max="5" width="13" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="28" t="s">
+      <c r="C3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="D3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="E3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="18" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="19">
-        <v>1</v>
-      </c>
-      <c r="C4" s="19">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19">
-        <v>3</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -949,66 +950,79 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="11" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" style="11" customWidth="1" collapsed="1"/>
-    <col min="3" max="8" width="14" style="11" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14" style="11" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="8.42578125" style="11"/>
+    <col min="1" max="1" width="9" style="10" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" style="10" customWidth="1" collapsed="1"/>
+    <col min="3" max="8" width="14" style="10" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" style="10" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="8.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
-        <v>30</v>
-      </c>
+      <c r="A1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1019,7 +1033,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,72 +1050,72 @@
     <col min="11" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1117,7 +1131,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,87 +1145,87 @@
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="32" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32" t="s">
+      <c r="D3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="23" t="s">
+      <c r="E3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="F3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18">
+        <v>3</v>
+      </c>
+      <c r="D4" s="18">
+        <v>4</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="F4" s="18">
+        <v>6</v>
+      </c>
+      <c r="G4" s="18">
+        <v>7</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
-        <v>1</v>
-      </c>
-      <c r="B4" s="21">
-        <v>2</v>
-      </c>
-      <c r="C4" s="22">
-        <v>3</v>
-      </c>
-      <c r="D4" s="22">
-        <v>4</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="22">
-        <v>6</v>
-      </c>
-      <c r="G4" s="22">
-        <v>7</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1245,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,100 +1264,117 @@
     <col min="15" max="17" width="14" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
-        <v>29</v>
-      </c>
+    <row r="1" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
     </row>
     <row r="3" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="38" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="37" t="s">
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="36" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="35" t="s">
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="26" t="s">
-        <v>40</v>
+      <c r="A4" s="31"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="O3:Q3"/>
@@ -1362,7 +1393,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,43 +1403,43 @@
     <col min="3" max="7" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1423,112 +1454,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE8E21-C3E8-4C2F-9589-406C158880E0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="41" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="34.85546875" style="41"/>
+    <col min="1" max="1" width="12.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="34.85546875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>1</v>
+      </c>
+      <c r="B4" s="24">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24">
+        <v>3</v>
+      </c>
+      <c r="D4" s="24">
+        <v>4</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="24">
+        <v>6</v>
+      </c>
+      <c r="G4" s="24">
+        <v>7</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
-        <v>1</v>
-      </c>
-      <c r="B4" s="44">
-        <v>2</v>
-      </c>
-      <c r="C4" s="44">
-        <v>3</v>
-      </c>
-      <c r="D4" s="44">
-        <v>4</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="44">
-        <v>6</v>
-      </c>
-      <c r="G4" s="44">
-        <v>7</v>
-      </c>
-      <c r="H4" s="44" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
+      <c r="A5" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1547,7 +1578,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,105 +1588,232 @@
     <col min="3" max="9" width="14" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>34</v>
+      <c r="A4" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="57" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="23" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+    </row>
+    <row r="3" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" s="42"/>
+      <c r="W3" s="42"/>
+    </row>
+    <row r="4" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4" s="41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bcThang => Sửa sai tí tỷ lệ nội trú vùng ở PL02x
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF7F16A-B3B8-4D4E-8959-F1B6CC775D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F016D2DC-743E-4132-A232-D9B740E6EFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
   <si>
     <t>Mã Tỉnh</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Hạng BV/ Tên CSKCB</t>
+  </si>
+  <si>
+    <t>Chi KCB (ĐVT: Triệu đồng)</t>
   </si>
 </sst>
 </file>
@@ -476,9 +479,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -494,13 +494,25 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -523,6 +535,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -530,15 +545,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -547,9 +553,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -570,9 +573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -610,7 +613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -716,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -858,7 +861,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -869,7 +872,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -882,19 +885,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -965,19 +968,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1051,19 +1054,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -1079,37 +1082,37 @@
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1130,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A251F88-94E1-426D-A092-C2C18E33BFDB}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,54 +1149,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="19" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="27" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1265,105 +1268,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
     </row>
     <row r="3" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35" t="s">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="34" t="s">
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="33" t="s">
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="32" t="s">
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="22" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="22" t="s">
+      <c r="P4" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1404,36 +1407,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1460,106 +1463,106 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="34.85546875" style="23"/>
+    <col min="1" max="1" width="12.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="34.85546875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="24" t="s">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
+      <c r="A4" s="23">
         <v>1</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>2</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>3</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>6</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>7</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1589,17 +1592,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1647,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1660,139 +1663,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
     </row>
     <row r="3" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42" t="s">
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42" t="s">
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42" t="s">
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42" t="s">
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42" t="s">
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-    </row>
-    <row r="4" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="41" t="s">
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="41" t="s">
+      <c r="K4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="41" t="s">
+      <c r="M4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="41" t="s">
+      <c r="N4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="41" t="s">
+      <c r="O4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="41" t="s">
+      <c r="Q4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="R4" s="41" t="s">
+      <c r="R4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="S4" s="41" t="s">
+      <c r="S4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="41" t="s">
+      <c r="T4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="U4" s="41" t="s">
+      <c r="U4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="41" t="s">
+      <c r="V4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="41" t="s">
+      <c r="W4" s="26" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bcThang => PL03 đã cập nhật Vùng tháng trước
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F016D2DC-743E-4132-A232-D9B740E6EFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8A8A8-9F98-4D55-9D2E-150E5BF0F260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="47">
   <si>
     <t>Mã Tỉnh</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lượt KCB </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chi KCB </t>
   </si>
   <si>
     <t>Năm nay</t>
@@ -1055,7 +1052,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1133,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A251F88-94E1-426D-A092-C2C18E33BFDB}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1170,7 @@
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
       <c r="F2" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
@@ -1182,22 +1179,22 @@
       <c r="A3" s="31"/>
       <c r="B3" s="31"/>
       <c r="C3" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>38</v>
-      </c>
       <c r="F3" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="H3" s="27" t="s">
         <v>37</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1214,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="18">
         <v>6</v>
@@ -1223,7 +1220,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1325,49 +1322,49 @@
       <c r="A4" s="34"/>
       <c r="B4" s="33"/>
       <c r="C4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="E4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="H4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="K4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="N4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="Q4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1408,7 +1405,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1457,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE8E21-C3E8-4C2F-9589-406C158880E0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1473,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -1498,32 +1495,32 @@
       </c>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
-      <c r="F2" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="F2" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>43</v>
-      </c>
       <c r="E3" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>43</v>
-      </c>
       <c r="H3" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1540,7 +1537,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="23">
         <v>6</v>
@@ -1549,7 +1546,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1694,7 +1691,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>7</v>
@@ -1736,67 +1733,67 @@
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="E4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="H4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="K4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="N4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="Q4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="S4" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="T4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="W4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bcThang => PL .xlsx định dạng số theo VN-VI
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8A8A8-9F98-4D55-9D2E-150E5BF0F260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B04197E-72F3-4D9B-B012-88A2975ED2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -1454,7 +1454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE8E21-C3E8-4C2F-9589-406C158880E0}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
@@ -1647,7 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bcThang => Chỉnh bcthangdocx, PL02c,Pl03c sắp xếp theo mã cha
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B04197E-72F3-4D9B-B012-88A2975ED2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3C892B-EB24-4392-9B66-A0D7A89732CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
   <si>
     <t>Mã Tỉnh</t>
   </si>
@@ -147,12 +147,6 @@
     <t>tăng/giảm</t>
   </si>
   <si>
-    <t>5=3-4</t>
-  </si>
-  <si>
-    <t>8=6-7</t>
-  </si>
-  <si>
     <t>So sánh lượt KCB và chi KCB tháng này với tháng trước</t>
   </si>
   <si>
@@ -172,6 +166,15 @@
   </si>
   <si>
     <t>Chi KCB (ĐVT: Triệu đồng)</t>
+  </si>
+  <si>
+    <t>6=4-5</t>
+  </si>
+  <si>
+    <t>9=7-8</t>
+  </si>
+  <si>
+    <t>Mã cấp trên</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -489,14 +492,15 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,6 +516,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -550,6 +560,11 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -882,19 +897,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="29"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -965,19 +980,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1051,19 +1066,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="A1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -1128,113 +1143,123 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A251F88-94E1-426D-A092-C2C18E33BFDB}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H2"/>
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="27" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="G3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="I3" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>1</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="26">
         <v>2</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>3</v>
       </c>
       <c r="D4" s="18">
         <v>4</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="18">
-        <v>6</v>
+      <c r="E4" s="18">
+        <v>5</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="G4" s="18">
         <v>7</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="18">
+        <v>8</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1265,103 +1290,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
     </row>
     <row r="3" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="38" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="37" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="36" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="35" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="21" t="s">
         <v>37</v>
@@ -1404,15 +1429,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="A1" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1452,122 +1477,133 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE8E21-C3E8-4C2F-9589-406C158880E0}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="34.85546875" style="22"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="34.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="42"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="32" t="s">
+      <c r="F3" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26">
+        <v>2</v>
+      </c>
+      <c r="C4" s="26">
+        <v>3</v>
+      </c>
+      <c r="D4" s="49">
+        <v>4</v>
+      </c>
+      <c r="E4" s="49">
+        <v>5</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="49">
+        <v>7</v>
+      </c>
+      <c r="H4" s="49">
+        <v>8</v>
+      </c>
+      <c r="I4" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
-        <v>1</v>
-      </c>
-      <c r="B4" s="23">
-        <v>2</v>
-      </c>
-      <c r="C4" s="23">
-        <v>3</v>
-      </c>
-      <c r="D4" s="23">
-        <v>4</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="23">
-        <v>6</v>
-      </c>
-      <c r="G4" s="23">
-        <v>7</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1589,17 +1625,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1647,7 +1683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1660,139 +1696,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
     </row>
     <row r="3" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43" t="s">
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43" t="s">
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43" t="s">
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43" t="s">
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43" t="s">
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="26" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="26" t="s">
+      <c r="F4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="26" t="s">
+      <c r="I4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="26" t="s">
+      <c r="L4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="26" t="s">
+      <c r="O4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="T4" s="26" t="s">
+      <c r="R4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="U4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="V4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="W4" s="26" t="s">
+      <c r="U4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="24" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bcThang => Thêm mã cha PL03a-b, PL04b
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/bcThangPL.xlsx
+++ b/ToolBaoCao/App_Data/bcThangPL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3C892B-EB24-4392-9B66-A0D7A89732CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEF5DA5-C969-4D60-8B00-3D24E0A84650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="49">
   <si>
     <t>Mã Tỉnh</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Mã cấp trên</t>
+  </si>
+  <si>
+    <t>Mã cha</t>
   </si>
 </sst>
 </file>
@@ -501,6 +504,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,10 +568,8 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -897,19 +902,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="28"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -980,19 +985,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1066,19 +1071,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -1162,43 +1167,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="30"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="25" t="s">
         <v>35</v>
       </c>
@@ -1267,146 +1272,152 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="14" customWidth="1"/>
-    <col min="15" max="17" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="14" customWidth="1"/>
+    <col min="16" max="18" width="14" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-    </row>
-    <row r="3" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+    </row>
+    <row r="3" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="C3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="D3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="39" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="38" t="s">
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="36" t="s">
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="21" t="s">
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="I4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="K4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="L4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="M4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="N4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="O4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="P4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="Q4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="R4" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:Q1"/>
+  <mergeCells count="9">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1415,61 +1426,64 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CADD43-DD89-4EFF-BE3D-EA660AB37B64}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="7" width="17.28515625" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="8" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-    </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="C3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="D3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1479,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FE8E21-C3E8-4C2F-9589-406C158880E0}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
@@ -1498,43 +1512,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="31" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="42"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="23" t="s">
         <v>39</v>
       </c>
@@ -1564,37 +1578,36 @@
       <c r="C4" s="26">
         <v>3</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="28">
         <v>4</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="28">
         <v>5</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="49">
+      <c r="G4" s="28">
         <v>7</v>
       </c>
-      <c r="H4" s="49">
+      <c r="H4" s="28">
         <v>8</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1625,17 +1638,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1681,174 +1694,180 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="57" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="23" width="15.28515625" customWidth="1"/>
+    <col min="1" max="2" width="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="57" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="24" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-    </row>
-    <row r="3" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+    </row>
+    <row r="3" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="C3" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="D3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44" t="s">
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44" t="s">
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44" t="s">
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44" t="s">
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="24" t="s">
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="F4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="G4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="H4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="I4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="J4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="K4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="L4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="M4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="N4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="O4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="P4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="Q4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="R4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="S4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="T4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="24" t="s">
+      <c r="U4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="V4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="W4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="24" t="s">
+      <c r="X4" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>32</v>
       </c>
+      <c r="B5" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="U3:W3"/>
+  <mergeCells count="11">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="B1:X1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>